<commit_message>
add area to Q files stn4
</commit_message>
<xml_diff>
--- a/Discharge/Station3_2021-06-14_1116.xlsx
+++ b/Discharge/Station3_2021-06-14_1116.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tessamd\Desktop\Ecuador Discharge\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1cba20500feb7d90/Documents/LongTermData_CayambeCoca/Discharge/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_D29837D5EA93E51F5FD15228D10DA985C0B5A9DB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3EE6987-3CDD-479D-BAE8-1185367E10C2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14640" windowHeight="9730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>h1</t>
   </si>
@@ -39,12 +49,21 @@
   </si>
   <si>
     <t>Q</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Atotal</t>
+  </si>
+  <si>
+    <t>Qtotal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,11 +374,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A11" sqref="A11:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,6 +436,33 @@
         <v>5.1240000000000009E-3</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <f>(C2+C3)/2*C4</f>
+        <v>4.2000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <f>B8</f>
+        <v>4.2000000000000006E-3</v>
+      </c>
+      <c r="B11">
+        <f>B7</f>
+        <v>5.1240000000000009E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>